<commit_message>
Moving Indexing to match Firestore
</commit_message>
<xml_diff>
--- a/pure/wingbank_faqs.xlsx
+++ b/pure/wingbank_faqs.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakhim.chea/PythonProjects/GeniusDaughter/pure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98003AE8-7F37-1B4B-9327-98B46A270120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D0ECE4-A325-454D-AE2A-0F3EA8EEDE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wingbank_faqs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="334">
   <si>
     <t>What is Wing Digital Loan?</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Does interest payment pay by month?</t>
   </si>
   <si>
-    <t>Yes, it does.</t>
-  </si>
-  <si>
     <t>How many term deposit accounts can I open?</t>
   </si>
   <si>
@@ -724,18 +721,9 @@
     <t>Response EN</t>
   </si>
   <si>
-    <t>Application by Wing agent</t>
-  </si>
-  <si>
-    <t>Extra fee charged from applications by Wing agent</t>
-  </si>
-  <si>
     <t>Does this loan service require collateral or guarantor?</t>
   </si>
   <si>
-    <t>Wing bank Visa debit card</t>
-  </si>
-  <si>
     <t>Wing bank Visa debit card eligibility</t>
   </si>
   <si>
@@ -745,192 +733,30 @@
     <t>What should I do to get OTP for my online transaction if I am abroad or if my phone cannot receive OTP?</t>
   </si>
   <si>
-    <t>Loan interest rate</t>
-  </si>
-  <si>
-    <t>Loan tenure</t>
-  </si>
-  <si>
-    <t>Maximum loan amount</t>
-  </si>
-  <si>
-    <t>Collateral or guarantor by loan service</t>
-  </si>
-  <si>
-    <t>Card renewal</t>
-  </si>
-  <si>
-    <t>Online payment or request OTP</t>
-  </si>
-  <si>
-    <t>Account overcharged</t>
-  </si>
-  <si>
-    <t>Forget pin or reset pin or change pin</t>
-  </si>
-  <si>
     <t>Wing Visa debit card validity</t>
   </si>
   <si>
-    <t>Offer credit limits to cardholders</t>
-  </si>
-  <si>
-    <t>The documents to apply for credit card</t>
-  </si>
-  <si>
-    <t>The ways to apply for credit card</t>
-  </si>
-  <si>
     <t>Wing bank Visa credit card eligibility or credit card eligibility</t>
   </si>
   <si>
-    <t>The benefits of Visa credit Gold and Platinum</t>
-  </si>
-  <si>
-    <t>Types of Visa credit card</t>
-  </si>
-  <si>
-    <t>Visa credit card</t>
-  </si>
-  <si>
-    <t>A joint account for Visa card</t>
-  </si>
-  <si>
-    <t>Stolen or lost card or Visa card resolutions</t>
-  </si>
-  <si>
-    <t>digital loan</t>
-  </si>
-  <si>
     <t>digital loan eligibility</t>
   </si>
   <si>
     <t>digital loan application</t>
   </si>
   <si>
-    <t>Reason to apply digital loan</t>
-  </si>
-  <si>
-    <t>Visa credit card without a bank account</t>
-  </si>
-  <si>
     <t>Visa card validity</t>
   </si>
   <si>
-    <t>Withdrawal amount from credit card</t>
-  </si>
-  <si>
-    <t>The ways to open a Saving account</t>
-  </si>
-  <si>
-    <t>The benefits of a saving account</t>
-  </si>
-  <si>
-    <t>The maximum transfer limit per day</t>
-  </si>
-  <si>
-    <t>The maximum transfer limit per transaction</t>
-  </si>
-  <si>
-    <t>The interest rate of a saving account</t>
-  </si>
-  <si>
-    <t>A fee for a new account</t>
-  </si>
-  <si>
-    <t>Saving account deposit</t>
-  </si>
-  <si>
-    <t>Saving account withdrawal</t>
-  </si>
-  <si>
-    <t>Fee to close an account</t>
-  </si>
-  <si>
-    <t>Interest paid monthly</t>
-  </si>
-  <si>
-    <t>The number of term deposit accounts</t>
-  </si>
-  <si>
-    <t>A certificate of term deposit</t>
-  </si>
-  <si>
-    <t>They way to know the interest amount is paid</t>
-  </si>
-  <si>
-    <t>Old deposit account with new interest rate</t>
-  </si>
-  <si>
-    <t>Closing term deposit accounts before the maturity date</t>
-  </si>
-  <si>
-    <t>The maximum transfer limit per day of saving account</t>
-  </si>
-  <si>
-    <t>The maximum transfer limit per transaction of saving account</t>
-  </si>
-  <si>
-    <t>The interest rate of a current account</t>
-  </si>
-  <si>
-    <t>The way to open an account</t>
-  </si>
-  <si>
-    <t>Reason to use agency</t>
-  </si>
-  <si>
     <t>Where can I perform my cash-in-out service?</t>
   </si>
   <si>
-    <t>Locations of agencies</t>
-  </si>
-  <si>
-    <t>To cash in or cash out with Bakong</t>
-  </si>
-  <si>
-    <t>The way to cash in or cash out with an agency</t>
-  </si>
-  <si>
-    <t>Number of cash in or cash out per day</t>
-  </si>
-  <si>
-    <t>Receive money from abroad</t>
-  </si>
-  <si>
     <t>What is the requirement for Inward Remittance?</t>
   </si>
   <si>
-    <t>The requirement to receive money from abroad</t>
-  </si>
-  <si>
-    <t>The processing time to receive money from abroad</t>
-  </si>
-  <si>
-    <t>Wing address to receive money from abroad</t>
-  </si>
-  <si>
     <t>The maximum amount for Inward transfer is unlimited.</t>
   </si>
   <si>
-    <t>The maximum amount for inbound transfer</t>
-  </si>
-  <si>
-    <t>Countries to be accepted transfer to bank account</t>
-  </si>
-  <si>
-    <t>The way to reject or return money back</t>
-  </si>
-  <si>
-    <t>Zero fee or free transfer from abroad</t>
-  </si>
-  <si>
-    <t>A fee for international transfer</t>
-  </si>
-  <si>
-    <t>The way to do money transfer without app</t>
-  </si>
-  <si>
     <t>Question EN</t>
   </si>
   <si>
@@ -1111,12 +937,6 @@
     <t>តើអ្វីទៅជាអត្ថប្រយោជន៍នៃការប្រើប្រាស់ឥណទានវីសាកាតប្រភេទមាសនិងផ្លាទីន?</t>
   </si>
   <si>
-    <t>A current account to open a term deposit account</t>
-  </si>
-  <si>
-    <t>Notifications of transactions or transferring</t>
-  </si>
-  <si>
     <t>តើឯកសារដែលត្រូវការសម្រាប់ស្នើរសុំធ្វើឥណទានវិសាការធនាគារវីងមានអ្វីខ្លះ?</t>
   </si>
   <si>
@@ -1136,6 +956,192 @@
   </si>
   <si>
     <t>តើខ្ញុំអាចប្រើឥណពន្ធវីសាកាតធនាគារវីងដោយរបៀបណានិងនៅទីណា?</t>
+  </si>
+  <si>
+    <t>about digital loan</t>
+  </si>
+  <si>
+    <t>to apply application by Wing agent</t>
+  </si>
+  <si>
+    <t>extra fee charged from applications by Wing agent</t>
+  </si>
+  <si>
+    <t>about loan interest rate</t>
+  </si>
+  <si>
+    <t>reasons to apply digital loan</t>
+  </si>
+  <si>
+    <t>about loan tenure</t>
+  </si>
+  <si>
+    <t>the maximum loan amount</t>
+  </si>
+  <si>
+    <t>the requirements of collateral or guarantor by loan service</t>
+  </si>
+  <si>
+    <t>about Wing bank Visa debit card</t>
+  </si>
+  <si>
+    <t>about card renewals</t>
+  </si>
+  <si>
+    <t>The resolutions to stolen or lost card or Visa card</t>
+  </si>
+  <si>
+    <t>about online payments or ways to request OTP</t>
+  </si>
+  <si>
+    <t>about account overcharged</t>
+  </si>
+  <si>
+    <t>to change or reset pin code</t>
+  </si>
+  <si>
+    <t>How can I change my PIN code?</t>
+  </si>
+  <si>
+    <t>the resolutions to forgotten pin code</t>
+  </si>
+  <si>
+    <t>about a joint account for Visa card</t>
+  </si>
+  <si>
+    <t>about Visa credit card</t>
+  </si>
+  <si>
+    <t>the types of Visa credit card</t>
+  </si>
+  <si>
+    <t>the benefits of Visa credit Gold and Platinum</t>
+  </si>
+  <si>
+    <t>the offer credit limits to cardholders</t>
+  </si>
+  <si>
+    <t>the documents to apply for credit card</t>
+  </si>
+  <si>
+    <t>the ways to apply for credit card</t>
+  </si>
+  <si>
+    <t>the possibility of Visa credit card without a bank account</t>
+  </si>
+  <si>
+    <t>the withdrawal amount from credit card</t>
+  </si>
+  <si>
+    <t>the ways to open a Saving account</t>
+  </si>
+  <si>
+    <t>the benefits of a saving account</t>
+  </si>
+  <si>
+    <t>the maximum transfer limit per day of a saving account</t>
+  </si>
+  <si>
+    <t>the maximum transfer limit per transaction of a saving account</t>
+  </si>
+  <si>
+    <t>the interest rate of a saving account</t>
+  </si>
+  <si>
+    <t>a fee for a new account</t>
+  </si>
+  <si>
+    <t>about saving account deposit</t>
+  </si>
+  <si>
+    <t>about saving account withdrawal</t>
+  </si>
+  <si>
+    <t>the fee to close an account</t>
+  </si>
+  <si>
+    <t>Yes, it does pay monthly.</t>
+  </si>
+  <si>
+    <t>how the interest is paid</t>
+  </si>
+  <si>
+    <t>the number of term deposit accounts to be opened</t>
+  </si>
+  <si>
+    <t>a certificate of term deposit</t>
+  </si>
+  <si>
+    <t>a current account to open a term deposit account</t>
+  </si>
+  <si>
+    <t>the way to know when the interest amount is paid</t>
+  </si>
+  <si>
+    <t>old deposit account with new interest rate</t>
+  </si>
+  <si>
+    <t>about closing term deposit accounts before the maturity date</t>
+  </si>
+  <si>
+    <t>the maximum transfer limit per transaction</t>
+  </si>
+  <si>
+    <t>the interest rate of a current account</t>
+  </si>
+  <si>
+    <t>the maximum transfer limit per day</t>
+  </si>
+  <si>
+    <t>the way to open an account</t>
+  </si>
+  <si>
+    <t>reason to resolute with agency</t>
+  </si>
+  <si>
+    <t>the locations of agencies</t>
+  </si>
+  <si>
+    <t>to cash in or cash out with Bakong</t>
+  </si>
+  <si>
+    <t>the way to cash in or cash out with an agency</t>
+  </si>
+  <si>
+    <t>the number of transactions per day via Bakong</t>
+  </si>
+  <si>
+    <t>about receiving money from abroad</t>
+  </si>
+  <si>
+    <t>the requirements to receive money from abroad</t>
+  </si>
+  <si>
+    <t>the processing time to receive money from abroad</t>
+  </si>
+  <si>
+    <t>the Wing address to receive money from abroad</t>
+  </si>
+  <si>
+    <t>the maximum amount for inbound transfer</t>
+  </si>
+  <si>
+    <t>the countries to be accepted transfer to bank account</t>
+  </si>
+  <si>
+    <t>the way to reject or return money back</t>
+  </si>
+  <si>
+    <t>the way to get zero fee or free transfer from abroad</t>
+  </si>
+  <si>
+    <t>about the fee for international transfer</t>
+  </si>
+  <si>
+    <t>the notifications of transactions or transferring</t>
+  </si>
+  <si>
+    <t>the way to do money transfer without app</t>
   </si>
 </sst>
 </file>
@@ -2011,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2026,36 +2032,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>263</v>
+        <v>205</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>264</v>
+        <v>206</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="64">
+    </row>
+    <row r="2" spans="1:5" ht="60">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>265</v>
+        <v>207</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>219</v>
+        <v>272</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2063,16 +2069,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>266</v>
+        <v>208</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2080,16 +2086,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>267</v>
+        <v>209</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2097,16 +2103,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>268</v>
+        <v>210</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>194</v>
+        <v>273</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2114,16 +2120,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>269</v>
+        <v>211</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>195</v>
+        <v>274</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2131,50 +2137,50 @@
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>270</v>
+        <v>212</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>222</v>
+        <v>276</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>271</v>
+        <v>213</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>201</v>
+        <v>275</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="32">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>272</v>
+        <v>214</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>202</v>
+        <v>277</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2182,50 +2188,50 @@
         <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>273</v>
+        <v>215</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>274</v>
+        <v>216</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="80">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="75">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>275</v>
+        <v>217</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>197</v>
+        <v>280</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2233,84 +2239,84 @@
         <v>21</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="48">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>331</v>
+        <v>271</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="32">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>277</v>
+        <v>219</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>205</v>
+        <v>281</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="32">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>278</v>
+        <v>220</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>218</v>
+        <v>282</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="48">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45">
       <c r="A17" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>279</v>
+        <v>221</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>206</v>
+        <v>283</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2318,866 +2324,883 @@
         <v>30</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>280</v>
+        <v>222</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>207</v>
+        <v>284</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>286</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>281</v>
+        <v>223</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="B21" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="48">
-      <c r="A21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="1" t="s">
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="48">
-      <c r="A22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="1" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="1" t="s">
+    <row r="25" spans="1:5" ht="240">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="51">
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="256">
-      <c r="A24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="1" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="289">
+      <c r="A28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="51">
-      <c r="A25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="1" t="s">
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="289">
-      <c r="A27" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="32">
-      <c r="A28" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="1" t="s">
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="32">
-      <c r="A29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="B32" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="153">
+      <c r="A33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="238">
+      <c r="A34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="153">
-      <c r="A32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="238">
-      <c r="A33" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="32">
-      <c r="A34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="32">
-      <c r="A35" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="1" t="s">
+    <row r="37" spans="1:5" ht="51">
+      <c r="A37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="51">
-      <c r="A36" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="1" t="s">
+    <row r="38" spans="1:5">
+      <c r="A38" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="2" t="s">
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="32">
-      <c r="A38" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="1" t="s">
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="32">
-      <c r="A39" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>300</v>
+        <v>74</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>241</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>235</v>
+        <v>305</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>155</v>
+        <v>75</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="E43" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30">
+      <c r="A45" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30">
+      <c r="A46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30">
+      <c r="A47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="90">
+      <c r="A48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30">
+      <c r="A50" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="C50" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="153">
+      <c r="A52" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="32">
-      <c r="A43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="8" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="32">
-      <c r="A44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="D53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30">
+      <c r="A55" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30">
+      <c r="A58" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45">
+      <c r="A59" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="32">
-      <c r="A45" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="32">
-      <c r="A46" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="96">
-      <c r="A47" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="32">
-      <c r="A48" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="32">
-      <c r="A49" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="153">
-      <c r="A51" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="32">
-      <c r="A53" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32">
-      <c r="A54" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="32">
-      <c r="A55" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32">
-      <c r="A56" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="32">
-      <c r="A57" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="D59" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="48">
-      <c r="A58" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D60" s="4" t="s">
+      <c r="E61" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="B62" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="32">
-      <c r="A61" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D63" s="4" t="s">
+      <c r="E64" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="45">
+      <c r="A65" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="B65" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="48">
-      <c r="A64" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" s="8" t="s">
+    <row r="66" spans="1:5" ht="51">
+      <c r="A66" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="D66" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="17">
+      <c r="A67" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="51">
-      <c r="A65" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="17">
-      <c r="A66" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D66" s="4" t="s">
+    <row r="68" spans="1:5" ht="34">
+      <c r="A68" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="B68" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="34">
-      <c r="A67" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D67" s="4" t="s">
+    <row r="69" spans="1:5" ht="17">
+      <c r="A69" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="B69" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="17">
-      <c r="A68" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>